<commit_message>
tested 71 generic docs
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huytran/medullusproj/bc-network/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD06EECF-D4EF-7B48-8923-0862648DCE2E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAA56E6-687D-1D47-B03F-CD113DFA3BFA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2840" yWindow="2400" windowWidth="28040" windowHeight="16100" xr2:uid="{2BF53832-C986-7A47-9320-721C73914E25}"/>
+    <workbookView xWindow="420" yWindow="2100" windowWidth="28040" windowHeight="16100" activeTab="3" xr2:uid="{2BF53832-C986-7A47-9320-721C73914E25}"/>
   </bookViews>
   <sheets>
     <sheet name="EntityMaster" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="214">
   <si>
     <t>Sub Name</t>
   </si>
@@ -715,7 +715,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -725,6 +725,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -741,7 +765,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -801,6 +825,9 @@
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -811,6 +838,75 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1128,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53870B3-DF20-8645-85A1-7C27099D4F15}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD21"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1651,16 +1747,16 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1722,16 +1818,16 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1746,7 +1842,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2088,39 +2184,39 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="43" t="s">
         <v>159</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="44">
         <v>23598</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="48">
         <v>1000</v>
       </c>
-      <c r="H10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="10">
+      <c r="H10" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="49">
         <v>100</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="48">
         <f t="shared" si="0"/>
         <v>100000</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="K10" s="44" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2269,11 +2365,11 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
     </row>
   </sheetData>
   <sortState ref="A2:K14">
@@ -2283,15 +2379,16 @@
     <mergeCell ref="A16:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA0A66D-AFE8-1D4E-B822-F6BC299C91B9}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2300,7 +2397,7 @@
     <col min="2" max="2" width="5.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.1640625" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="8" customWidth="1"/>
     <col min="6" max="6" width="8.1640625" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.1640625" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.1640625" style="8" bestFit="1" customWidth="1"/>
@@ -2453,110 +2550,110 @@
         <v>36000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="43" t="s">
         <v>175</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="45">
         <v>43103</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="46">
         <v>1354651</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="44">
         <v>654864</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="49">
         <v>100</v>
       </c>
-      <c r="I5" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="10">
+      <c r="I5" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="49">
         <v>200</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="48">
         <f t="shared" si="0"/>
         <v>20000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="34">
         <v>43103</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="33">
         <v>1354651</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="57">
         <v>12345</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="58">
         <v>100</v>
       </c>
-      <c r="I6" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="10">
+      <c r="I6" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="58">
         <v>200</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="59">
         <f t="shared" si="0"/>
         <v>20000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="43" t="s">
         <v>171</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="45">
         <v>43103</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="46">
         <v>546568</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="44">
         <v>25412</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="49">
         <v>125</v>
       </c>
-      <c r="I7" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="10">
+      <c r="I7" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="49">
         <v>400</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="48">
         <f>H7*J7</f>
         <v>50000</v>
       </c>
@@ -2813,38 +2910,38 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="43" t="s">
         <v>182</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="45">
         <v>43120</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="46">
         <v>80203</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="46">
         <v>23598</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="47">
         <v>180</v>
       </c>
-      <c r="I15" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J15" s="15">
+      <c r="I15" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="47">
         <v>100</v>
       </c>
-      <c r="K15" s="11">
+      <c r="K15" s="48">
         <f t="shared" si="1"/>
         <v>18000</v>
       </c>
@@ -2885,7 +2982,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>186</v>
       </c>
@@ -2921,7 +3018,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>187</v>
       </c>
@@ -2957,7 +3054,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>188</v>
       </c>
@@ -2993,7 +3090,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>189</v>
       </c>
@@ -3029,7 +3126,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>190</v>
       </c>
@@ -3065,7 +3162,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>184</v>
       </c>
@@ -3101,12 +3198,99 @@
         <v>120000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="28" t="s">
+    <row r="24" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G29" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="H29" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="I29" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="J29" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="K29" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="L29" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="M29" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="N29" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="14">
+        <v>1354651</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" s="14">
+        <v>654864</v>
+      </c>
+      <c r="G30" s="15">
+        <v>100</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30" s="15">
+        <v>200</v>
+      </c>
+      <c r="J30" s="16">
+        <f t="shared" ref="J30" si="2">G30*I30</f>
+        <v>20000</v>
+      </c>
+      <c r="K30" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="L30" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14" t="s">
+        <v>87</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:K22">
@@ -3123,8 +3307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B7FC4D4-B9F9-0F44-A07C-C0D2E894A023}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3190,183 +3374,183 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:14" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="38">
         <v>80203</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="38">
         <v>23598</v>
       </c>
-      <c r="G2" s="15">
+      <c r="G2" s="39">
         <v>180</v>
       </c>
-      <c r="H2" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="15">
+      <c r="H2" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="39">
         <v>100</v>
       </c>
-      <c r="J2" s="16">
+      <c r="J2" s="40">
         <f>G2*I2</f>
         <v>18000</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="M2" s="13">
+      <c r="M2" s="41">
         <v>43125</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="38" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:14" s="56" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="50" t="s">
         <v>174</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="52">
         <v>1354651</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="52">
         <v>12345</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="53">
         <v>100</v>
       </c>
-      <c r="H3" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="15">
+      <c r="H3" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="53">
         <v>200</v>
       </c>
-      <c r="J3" s="16">
+      <c r="J3" s="54">
         <f t="shared" ref="J3:J7" si="0">G3*I3</f>
         <v>20000</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="L3" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="M3" s="13">
+      <c r="M3" s="55">
         <v>43105</v>
       </c>
-      <c r="N3" s="14" t="s">
+      <c r="N3" s="52" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:14" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="36" t="s">
         <v>171</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="38">
         <v>546568</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="38">
         <v>25412</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="39">
         <v>125</v>
       </c>
-      <c r="H4" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="15">
+      <c r="H4" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="39">
         <v>400</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="40">
         <f t="shared" si="0"/>
         <v>50000</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="L4" s="14" t="s">
+      <c r="L4" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="M4" s="13">
+      <c r="M4" s="41">
         <v>43122</v>
       </c>
-      <c r="N4" s="14" t="s">
+      <c r="N4" s="38" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:14" s="42" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="38">
         <v>56546</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="38">
         <v>23598</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="39">
         <v>150</v>
       </c>
-      <c r="H5" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="15">
+      <c r="H5" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="39">
         <v>100</v>
       </c>
-      <c r="J5" s="16">
+      <c r="J5" s="40">
         <f t="shared" si="0"/>
         <v>15000</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="L5" s="14" t="s">
+      <c r="L5" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="M5" s="13">
+      <c r="M5" s="41">
         <v>43118</v>
       </c>
-      <c r="N5" s="14" t="s">
+      <c r="N5" s="38" t="s">
         <v>83</v>
       </c>
     </row>
@@ -3457,129 +3641,129 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="30" t="s">
         <v>194</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="30" t="s">
         <v>191</v>
       </c>
-      <c r="B12" s="29"/>
+      <c r="B12" s="30"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="30" t="s">
         <v>193</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="30" t="s">
         <v>192</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="30" t="s">
         <v>197</v>
       </c>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="30" t="s">
         <v>196</v>
       </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="30" t="s">
         <v>195</v>
       </c>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
       <c r="F20" s="22"/>
       <c r="G20" s="22"/>
       <c r="H20" s="22"/>
@@ -3612,6 +3796,7 @@
     <mergeCell ref="A20:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3782,12 +3967,12 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="29" t="s">
         <v>204</v>
       </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3898,12 +4083,12 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4128,16 +4313,16 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4404,16 +4589,16 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4504,16 +4689,16 @@
       <c r="H3" s="18"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>